<commit_message>
Final changes; updated to save full boot of lambda, and not just the summary of the boot.
</commit_message>
<xml_diff>
--- a/Manuscripts/Results.xlsx
+++ b/Manuscripts/Results.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10123"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marina/Documents/UC-Davis/Manuscripts/Watering Experiment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marina/Documents/UC-Davis/Projects/McL_Climate-Competition/Manuscripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9630D1CA-E81B-F94C-977F-544E0D955CFA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F571FE-A0F3-3E4B-94D0-96372B9B2DEC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 2" sheetId="9" r:id="rId2"/>
-    <sheet name="Seed Set" sheetId="2" r:id="rId3"/>
-    <sheet name="Germination" sheetId="3" r:id="rId4"/>
-    <sheet name="Boot Lambda" sheetId="5" r:id="rId5"/>
-    <sheet name="Fig.1" sheetId="7" r:id="rId6"/>
-    <sheet name="Table 3" sheetId="10" r:id="rId7"/>
-    <sheet name="Table 1" sheetId="8" r:id="rId8"/>
+    <sheet name="Seed Set" sheetId="2" r:id="rId2"/>
+    <sheet name="Germination" sheetId="3" r:id="rId3"/>
+    <sheet name="Boot Lambda" sheetId="5" r:id="rId4"/>
+    <sheet name="Fig.1" sheetId="7" r:id="rId5"/>
+    <sheet name="Table 1" sheetId="8" r:id="rId6"/>
+    <sheet name="Table 2" sheetId="9" r:id="rId7"/>
+    <sheet name="Table 3" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -333,7 +333,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,6 +393,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1031,7 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="138" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="138" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -1062,11 +1085,11 @@
       <c r="D3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1337,819 +1360,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C15A15-B257-804A-B50E-116E7FBDD06F}">
-  <dimension ref="A1:G45"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:G46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="0.83203125" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" customWidth="1"/>
-    <col min="7" max="7" width="2.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
-      <c r="B2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="18">
-        <v>-1.0214300000000001</v>
-      </c>
-      <c r="C3" s="18">
-        <v>0.12503</v>
-      </c>
-      <c r="D3" s="18">
-        <v>-8.1690000000000005</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="18">
-        <v>0.27423999999999998</v>
-      </c>
-      <c r="C4" s="18">
-        <v>0.23208000000000001</v>
-      </c>
-      <c r="D4" s="18">
-        <v>1.1819999999999999</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="16">
-        <v>0.23733399999999999</v>
-      </c>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="18">
-        <v>-0.36484</v>
-      </c>
-      <c r="C5" s="18">
-        <v>0.17471999999999999</v>
-      </c>
-      <c r="D5" s="18">
-        <v>-2.0880000000000001</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="16">
-        <v>3.6789000000000002E-2</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="18">
-        <v>0.2152</v>
-      </c>
-      <c r="C6" s="18">
-        <v>8.1079999999999999E-2</v>
-      </c>
-      <c r="D6" s="18">
-        <v>2.6539999999999999</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="16">
-        <v>7.9539999999999993E-3</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="18">
-        <v>0.82784999999999997</v>
-      </c>
-      <c r="C7" s="18">
-        <v>0.10652</v>
-      </c>
-      <c r="D7" s="18">
-        <v>7.7720000000000002</v>
-      </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="16">
-        <v>7.7500000000000001E-15</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="18">
-        <v>0.39881</v>
-      </c>
-      <c r="C8" s="18">
-        <v>0.13411999999999999</v>
-      </c>
-      <c r="D8" s="18">
-        <v>2.9729999999999999</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="16">
-        <v>2.9450000000000001E-3</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="18">
-        <v>2.3099999999999999E-2</v>
-      </c>
-      <c r="C9" s="18">
-        <v>0.11445</v>
-      </c>
-      <c r="D9" s="18">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="16">
-        <v>0.84008400000000005</v>
-      </c>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="18">
-        <v>-0.72923000000000004</v>
-      </c>
-      <c r="C10" s="18">
-        <v>0.20294999999999999</v>
-      </c>
-      <c r="D10" s="18">
-        <v>-3.593</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="18">
-        <v>-0.38185999999999998</v>
-      </c>
-      <c r="C11" s="18">
-        <v>0.14888999999999999</v>
-      </c>
-      <c r="D11" s="18">
-        <v>-2.5649999999999999</v>
-      </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="16">
-        <v>1.0323000000000001E-2</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="18">
-        <v>3.9690000000000003E-2</v>
-      </c>
-      <c r="C12" s="18">
-        <v>7.2470000000000007E-2</v>
-      </c>
-      <c r="D12" s="18">
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="16">
-        <v>0.58393200000000001</v>
-      </c>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="18">
-        <v>0.21023</v>
-      </c>
-      <c r="C13" s="18">
-        <v>0.12511</v>
-      </c>
-      <c r="D13" s="18">
-        <v>1.68</v>
-      </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="16">
-        <v>9.2888999999999999E-2</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="19">
-        <v>0.25313999999999998</v>
-      </c>
-      <c r="C14" s="19">
-        <v>0.1022</v>
-      </c>
-      <c r="D14" s="19">
-        <v>2.4769999999999999</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="17">
-        <v>1.3251000000000001E-2</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="18">
-        <v>2.8773399999999998</v>
-      </c>
-      <c r="C19" s="18">
-        <v>9.0749999999999997E-2</v>
-      </c>
-      <c r="D19" s="18">
-        <v>31.706</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="18">
-        <v>0.43890000000000001</v>
-      </c>
-      <c r="C20" s="18">
-        <v>0.1729</v>
-      </c>
-      <c r="D20" s="18">
-        <v>2.5379999999999998</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="16">
-        <v>1.155E-2</v>
-      </c>
-      <c r="G20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="18">
-        <v>0.10201</v>
-      </c>
-      <c r="C21" s="18">
-        <v>0.12542</v>
-      </c>
-      <c r="D21" s="18">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="16">
-        <v>0.41652</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="18">
-        <v>-0.36897999999999997</v>
-      </c>
-      <c r="C22" s="18">
-        <v>8.8620000000000004E-2</v>
-      </c>
-      <c r="D22" s="18">
-        <v>-4.1639999999999997</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="18">
-        <v>-0.22731999999999999</v>
-      </c>
-      <c r="C23" s="18">
-        <v>7.0349999999999996E-2</v>
-      </c>
-      <c r="D23" s="18">
-        <v>-3.2309999999999999</v>
-      </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="16">
-        <v>1.3699999999999999E-3</v>
-      </c>
-      <c r="G23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="18">
-        <v>-0.48254999999999998</v>
-      </c>
-      <c r="C24" s="18">
-        <v>0.17011999999999999</v>
-      </c>
-      <c r="D24" s="18">
-        <v>-2.8359999999999999</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="16">
-        <v>4.96E-3</v>
-      </c>
-      <c r="G24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="18">
-        <v>-6.7140000000000005E-2</v>
-      </c>
-      <c r="C25" s="18">
-        <v>0.12242</v>
-      </c>
-      <c r="D25" s="18">
-        <v>-0.54800000000000004</v>
-      </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="16">
-        <v>0.58394000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="18">
-        <v>0.25152000000000002</v>
-      </c>
-      <c r="C26" s="18">
-        <v>0.13313</v>
-      </c>
-      <c r="D26" s="18">
-        <v>1.889</v>
-      </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="16">
-        <v>6.003E-2</v>
-      </c>
-      <c r="G26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="18">
-        <v>-6.1830000000000003E-2</v>
-      </c>
-      <c r="C27" s="18">
-        <v>9.214E-2</v>
-      </c>
-      <c r="D27" s="18">
-        <v>-0.67100000000000004</v>
-      </c>
-      <c r="E27" s="18"/>
-      <c r="F27" s="16">
-        <v>0.50280000000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="19">
-        <v>0.13120000000000001</v>
-      </c>
-      <c r="C28" s="19">
-        <v>4.8189999999999997E-2</v>
-      </c>
-      <c r="D28" s="19">
-        <v>2.722</v>
-      </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="17">
-        <v>6.9699999999999996E-3</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
-      <c r="B33" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="18">
-        <v>2.0674459999999999</v>
-      </c>
-      <c r="C34" s="18">
-        <v>1.1842E-2</v>
-      </c>
-      <c r="D34" s="18">
-        <v>174.58600000000001</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="18">
-        <v>0.37662800000000002</v>
-      </c>
-      <c r="C35" s="18">
-        <v>1.6747000000000001E-2</v>
-      </c>
-      <c r="D35" s="18">
-        <v>22.489000000000001</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="18">
-        <v>0.206845</v>
-      </c>
-      <c r="C36" s="18">
-        <v>1.6747000000000001E-2</v>
-      </c>
-      <c r="D36" s="18">
-        <v>12.351000000000001</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="18">
-        <v>-0.38437100000000002</v>
-      </c>
-      <c r="C37" s="18">
-        <v>1.6747000000000001E-2</v>
-      </c>
-      <c r="D37" s="18">
-        <v>-22.951000000000001</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="18">
-        <v>-0.52149900000000005</v>
-      </c>
-      <c r="C38" s="18">
-        <v>9.6080000000000002E-3</v>
-      </c>
-      <c r="D38" s="18">
-        <v>-54.277999999999999</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F38" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="18">
-        <v>-0.56345299999999998</v>
-      </c>
-      <c r="C39" s="18">
-        <v>2.3684E-2</v>
-      </c>
-      <c r="D39" s="18">
-        <v>-23.79</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="18">
-        <v>-7.8202999999999995E-2</v>
-      </c>
-      <c r="C40" s="18">
-        <v>2.3684E-2</v>
-      </c>
-      <c r="D40" s="18">
-        <v>-3.302</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="16">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="18">
-        <v>0.36754700000000001</v>
-      </c>
-      <c r="C41" s="18">
-        <v>1.3587999999999999E-2</v>
-      </c>
-      <c r="D41" s="18">
-        <v>27.05</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F41" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="18">
-        <v>4.0292000000000001E-2</v>
-      </c>
-      <c r="C42" s="18">
-        <v>1.3587999999999999E-2</v>
-      </c>
-      <c r="D42" s="18">
-        <v>2.9649999999999999</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="16">
-        <v>6.7400000000000003E-3</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="18">
-        <v>0.11838600000000001</v>
-      </c>
-      <c r="C43" s="18">
-        <v>1.3587999999999999E-2</v>
-      </c>
-      <c r="D43" s="18">
-        <v>8.7129999999999992</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F43" s="16">
-        <v>1E-3</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="18">
-        <v>-7.0462999999999998E-2</v>
-      </c>
-      <c r="C44" s="18">
-        <v>1.9216E-2</v>
-      </c>
-      <c r="D44" s="18">
-        <v>-3.6669999999999998</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="16">
-        <v>1.2199999999999999E-3</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="19">
-        <v>-4.2611000000000003E-2</v>
-      </c>
-      <c r="C45" s="19">
-        <v>1.9216E-2</v>
-      </c>
-      <c r="D45" s="19">
-        <v>-2.2170000000000001</v>
-      </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="17">
-        <v>3.6310000000000002E-2</v>
-      </c>
-      <c r="G45" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E33:G33"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
@@ -2184,11 +1394,11 @@
       <c r="D3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -2414,7 +1624,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -2504,12 +1714,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F15"/>
+      <selection activeCell="B4" sqref="B4:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2541,13 +1751,13 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>2.0674459999999999</v>
+        <v>2.06656</v>
       </c>
       <c r="C4">
-        <v>1.1842E-2</v>
+        <v>1.204E-2</v>
       </c>
       <c r="D4">
-        <v>174.58600000000001</v>
+        <v>171.619</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -2561,13 +1771,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.37662800000000002</v>
+        <v>0.38225999999999999</v>
       </c>
       <c r="C5">
-        <v>1.6747000000000001E-2</v>
+        <v>1.703E-2</v>
       </c>
       <c r="D5">
-        <v>22.489000000000001</v>
+        <v>22.446999999999999</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -2581,16 +1791,16 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0.206845</v>
+        <v>0.21387999999999999</v>
       </c>
       <c r="C6">
-        <v>1.6747000000000001E-2</v>
+        <v>1.703E-2</v>
       </c>
       <c r="D6">
-        <v>12.351000000000001</v>
+        <v>12.558999999999999</v>
       </c>
       <c r="E6" s="1">
-        <v>6.8600000000000003E-12</v>
+        <v>4.8400000000000004E-12</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
@@ -2601,13 +1811,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-0.38437100000000002</v>
+        <v>-0.38175999999999999</v>
       </c>
       <c r="C7">
-        <v>1.6747000000000001E-2</v>
+        <v>1.703E-2</v>
       </c>
       <c r="D7">
-        <v>-22.951000000000001</v>
+        <v>-22.417999999999999</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -2621,13 +1831,13 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-0.52149900000000005</v>
+        <v>-0.52281999999999995</v>
       </c>
       <c r="C8">
-        <v>9.6080000000000002E-3</v>
+        <v>9.7699999999999992E-3</v>
       </c>
       <c r="D8">
-        <v>-54.277999999999999</v>
+        <v>-53.512999999999998</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
@@ -2641,13 +1851,13 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-0.56345299999999998</v>
+        <v>-0.56810000000000005</v>
       </c>
       <c r="C9">
-        <v>2.3684E-2</v>
+        <v>2.4080000000000001E-2</v>
       </c>
       <c r="D9">
-        <v>-23.79</v>
+        <v>-23.588999999999999</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
@@ -2661,16 +1871,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>-7.8202999999999995E-2</v>
+        <v>-8.3099999999999993E-2</v>
       </c>
       <c r="C10">
-        <v>2.3684E-2</v>
+        <v>2.4080000000000001E-2</v>
       </c>
       <c r="D10">
-        <v>-3.302</v>
+        <v>-3.4510000000000001</v>
       </c>
       <c r="E10">
-        <v>3.0000000000000001E-3</v>
+        <v>2.0799999999999998E-3</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
@@ -2681,13 +1891,13 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.36754700000000001</v>
+        <v>0.37828000000000001</v>
       </c>
       <c r="C11">
-        <v>1.3587999999999999E-2</v>
+        <v>1.3820000000000001E-2</v>
       </c>
       <c r="D11">
-        <v>27.05</v>
+        <v>27.379000000000001</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
@@ -2701,16 +1911,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>4.0292000000000001E-2</v>
+        <v>3.9759999999999997E-2</v>
       </c>
       <c r="C12">
-        <v>1.3587999999999999E-2</v>
+        <v>1.3820000000000001E-2</v>
       </c>
       <c r="D12">
-        <v>2.9649999999999999</v>
+        <v>2.8780000000000001</v>
       </c>
       <c r="E12">
-        <v>6.7400000000000003E-3</v>
+        <v>8.2900000000000005E-3</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -2721,16 +1931,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0.11838600000000001</v>
+        <v>0.11841</v>
       </c>
       <c r="C13">
-        <v>1.3587999999999999E-2</v>
+        <v>1.3820000000000001E-2</v>
       </c>
       <c r="D13">
-        <v>8.7129999999999992</v>
+        <v>8.57</v>
       </c>
       <c r="E13" s="1">
-        <v>6.7500000000000001E-9</v>
+        <v>9.1399999999999995E-9</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
@@ -2741,16 +1951,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-7.0462999999999998E-2</v>
+        <v>-6.88E-2</v>
       </c>
       <c r="C14">
-        <v>1.9216E-2</v>
+        <v>1.9539999999999998E-2</v>
       </c>
       <c r="D14">
-        <v>-3.6669999999999998</v>
+        <v>-3.5209999999999999</v>
       </c>
       <c r="E14">
-        <v>1.2199999999999999E-3</v>
+        <v>1.75E-3</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
@@ -2761,19 +1971,19 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>-4.2611000000000003E-2</v>
+        <v>-3.9690000000000003E-2</v>
       </c>
       <c r="C15">
-        <v>1.9216E-2</v>
+        <v>1.9539999999999998E-2</v>
       </c>
       <c r="D15">
-        <v>-2.2170000000000001</v>
+        <v>-2.0310000000000001</v>
       </c>
       <c r="E15">
-        <v>3.6310000000000002E-2</v>
+        <v>5.3469999999999997E-2</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2787,7 +1997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA3020D-8CFE-8F4C-A1C1-3057A9F6B138}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2800,21 +2010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DBB117-98CE-A54A-914B-DEF81FDC56E7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED17359-1095-D542-A571-CB090B68E0B3}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -2983,4 +2179,968 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C15A15-B257-804A-B50E-116E7FBDD06F}">
+  <dimension ref="A1:H45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="0.83203125" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15"/>
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="18">
+        <v>-1.0214300000000001</v>
+      </c>
+      <c r="C3" s="18">
+        <v>0.12503</v>
+      </c>
+      <c r="D3" s="18">
+        <v>-8.1690000000000005</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.27423999999999998</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0.23208000000000001</v>
+      </c>
+      <c r="D4" s="18">
+        <v>1.1819999999999999</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="16">
+        <v>0.23733399999999999</v>
+      </c>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="18">
+        <v>-0.36484</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.17471999999999999</v>
+      </c>
+      <c r="D5" s="18">
+        <v>-2.0880000000000001</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="16">
+        <v>3.6789000000000002E-2</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="18">
+        <v>0.2152</v>
+      </c>
+      <c r="C6" s="18">
+        <v>8.1079999999999999E-2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2.6539999999999999</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="16">
+        <v>7.9539999999999993E-3</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="18">
+        <v>0.82784999999999997</v>
+      </c>
+      <c r="C7" s="18">
+        <v>0.10652</v>
+      </c>
+      <c r="D7" s="18">
+        <v>7.7720000000000002</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="16">
+        <v>7.7500000000000001E-15</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="18">
+        <v>0.39881</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.13411999999999999</v>
+      </c>
+      <c r="D8" s="18">
+        <v>2.9729999999999999</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="16">
+        <v>2.9450000000000001E-3</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2.3099999999999999E-2</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0.11445</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="16">
+        <v>0.84008400000000005</v>
+      </c>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="18">
+        <v>-0.72923000000000004</v>
+      </c>
+      <c r="C10" s="18">
+        <v>0.20294999999999999</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-3.593</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="18">
+        <v>-0.38185999999999998</v>
+      </c>
+      <c r="C11" s="18">
+        <v>0.14888999999999999</v>
+      </c>
+      <c r="D11" s="18">
+        <v>-2.5649999999999999</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="16">
+        <v>1.0323000000000001E-2</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="18">
+        <v>3.9690000000000003E-2</v>
+      </c>
+      <c r="C12" s="18">
+        <v>7.2470000000000007E-2</v>
+      </c>
+      <c r="D12" s="18">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="16">
+        <v>0.58393200000000001</v>
+      </c>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="18">
+        <v>0.21023</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0.12511</v>
+      </c>
+      <c r="D13" s="18">
+        <v>1.68</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="16">
+        <v>9.2888999999999999E-2</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="19">
+        <v>0.25313999999999998</v>
+      </c>
+      <c r="C14" s="19">
+        <v>0.1022</v>
+      </c>
+      <c r="D14" s="19">
+        <v>2.4769999999999999</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="17">
+        <v>1.3251000000000001E-2</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="18">
+        <v>2.8773399999999998</v>
+      </c>
+      <c r="C19" s="18">
+        <v>9.0749999999999997E-2</v>
+      </c>
+      <c r="D19" s="18">
+        <v>31.706</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="18">
+        <v>0.43890000000000001</v>
+      </c>
+      <c r="C20" s="18">
+        <v>0.1729</v>
+      </c>
+      <c r="D20" s="18">
+        <v>2.5379999999999998</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="16">
+        <v>1.155E-2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="18">
+        <v>0.10201</v>
+      </c>
+      <c r="C21" s="18">
+        <v>0.12542</v>
+      </c>
+      <c r="D21" s="18">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="16">
+        <v>0.41652</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="18">
+        <v>-0.36897999999999997</v>
+      </c>
+      <c r="C22" s="18">
+        <v>8.8620000000000004E-2</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-4.1639999999999997</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="18">
+        <v>-0.22731999999999999</v>
+      </c>
+      <c r="C23" s="18">
+        <v>7.0349999999999996E-2</v>
+      </c>
+      <c r="D23" s="18">
+        <v>-3.2309999999999999</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="16">
+        <v>1.3699999999999999E-3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="18">
+        <v>-0.48254999999999998</v>
+      </c>
+      <c r="C24" s="18">
+        <v>0.17011999999999999</v>
+      </c>
+      <c r="D24" s="18">
+        <v>-2.8359999999999999</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="16">
+        <v>4.96E-3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="18">
+        <v>-6.7140000000000005E-2</v>
+      </c>
+      <c r="C25" s="18">
+        <v>0.12242</v>
+      </c>
+      <c r="D25" s="18">
+        <v>-0.54800000000000004</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="16">
+        <v>0.58394000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="18">
+        <v>0.25152000000000002</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0.13313</v>
+      </c>
+      <c r="D26" s="18">
+        <v>1.889</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="16">
+        <v>6.003E-2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="18">
+        <v>-6.1830000000000003E-2</v>
+      </c>
+      <c r="C27" s="18">
+        <v>9.214E-2</v>
+      </c>
+      <c r="D27" s="18">
+        <v>-0.67100000000000004</v>
+      </c>
+      <c r="E27" s="18"/>
+      <c r="F27" s="16">
+        <v>0.50280000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="19">
+        <v>0.13120000000000001</v>
+      </c>
+      <c r="C28" s="19">
+        <v>4.8189999999999997E-2</v>
+      </c>
+      <c r="D28" s="19">
+        <v>2.722</v>
+      </c>
+      <c r="E28" s="19"/>
+      <c r="F28" s="17">
+        <v>6.9699999999999996E-3</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="21"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="22"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="38"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="22"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="38"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="22"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="22"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="38"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="22"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="38"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="22"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="38"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="22"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="38"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="22"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="38"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="22"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="38"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="22"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="22"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="38"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="22"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E33:G33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DBB117-98CE-A54A-914B-DEF81FDC56E7}">
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="0.83203125" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20"/>
+      <c r="B1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="18">
+        <v>2.06656</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1.204E-2</v>
+      </c>
+      <c r="D2" s="18">
+        <v>171.619</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="18">
+        <v>0.38225999999999999</v>
+      </c>
+      <c r="C3" s="18">
+        <v>1.703E-2</v>
+      </c>
+      <c r="D3" s="18">
+        <v>22.446999999999999</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.21387999999999999</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1.703E-2</v>
+      </c>
+      <c r="D4" s="18">
+        <v>12.558999999999999</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="18">
+        <v>-0.38175999999999999</v>
+      </c>
+      <c r="C5" s="18">
+        <v>1.703E-2</v>
+      </c>
+      <c r="D5" s="18">
+        <v>-22.417999999999999</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="18">
+        <v>-0.52281999999999995</v>
+      </c>
+      <c r="C6" s="18">
+        <v>9.7699999999999992E-3</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-53.512999999999998</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="18">
+        <v>-0.56810000000000005</v>
+      </c>
+      <c r="C7" s="18">
+        <v>2.4080000000000001E-2</v>
+      </c>
+      <c r="D7" s="18">
+        <v>-23.588999999999999</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="18">
+        <v>-8.3099999999999993E-2</v>
+      </c>
+      <c r="C8" s="18">
+        <v>2.4080000000000001E-2</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-3.4510000000000001</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="16">
+        <v>2E-3</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="18">
+        <v>0.37828000000000001</v>
+      </c>
+      <c r="C9" s="18">
+        <v>1.3820000000000001E-2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>27.379000000000001</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="18">
+        <v>3.9759999999999997E-2</v>
+      </c>
+      <c r="C10" s="18">
+        <v>1.3820000000000001E-2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>2.8780000000000001</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="16">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="18">
+        <v>0.11841</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1.3820000000000001E-2</v>
+      </c>
+      <c r="D11" s="18">
+        <v>8.57</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="18">
+        <v>-6.88E-2</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1.9539999999999998E-2</v>
+      </c>
+      <c r="D12" s="18">
+        <v>-3.5209999999999999</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="16">
+        <v>2E-3</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="19">
+        <v>-3.9690000000000003E-2</v>
+      </c>
+      <c r="C13" s="19">
+        <v>1.9539999999999998E-2</v>
+      </c>
+      <c r="D13" s="19">
+        <v>-2.0310000000000001</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="17">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>